<commit_message>
Updating example upload files and removing service contact funding source option 0. We have decided to keep that value in house.
</commit_message>
<xml_diff>
--- a/doc/data-specification/_data/_orig/headspace-clients-upload.xlsx
+++ b/doc/data-specification/_data/_orig/headspace-clients-upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenni/Work/git/PMHC/spec-headspace/data/_orig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5264A5A9-3B85-5046-947B-FBB7271F0CBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D07E598-BD22-EB42-89CF-EB0B6F973862}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42060" yWindow="3940" windowWidth="25360" windowHeight="15820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,10 +599,10 @@
     <t>continuity_of_support</t>
   </si>
   <si>
-    <t>headspace_funding_source</t>
-  </si>
-  <si>
     <t>delivery_organisation_path</t>
+  </si>
+  <si>
+    <t>funding_source</t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1573,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R6"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1631,10 +1631,10 @@
         <v>79</v>
       </c>
       <c r="Q1" t="s">
+        <v>189</v>
+      </c>
+      <c r="R1" t="s">
         <v>188</v>
-      </c>
-      <c r="R1" t="s">
-        <v>189</v>
       </c>
       <c r="S1" t="s">
         <v>80</v>
@@ -1795,7 +1795,7 @@
         <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G1" t="s">
         <v>85</v>
@@ -2146,7 +2146,7 @@
         <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G1" t="s">
         <v>105</v>
@@ -2368,7 +2368,7 @@
         <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G1" t="s">
         <v>116</v>

</xml_diff>